<commit_message>
verslag en afbeeldingen DLS
</commit_message>
<xml_diff>
--- a/Measurement_Results/DLS/Data_verslag/0.8.xlsx
+++ b/Measurement_Results/DLS/Data_verslag/0.8.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lies/Documents/Bachelorproef/Measurement_Results/DLS/Data_verslag/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="14360" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
   <si>
     <t>Acq N°1</t>
   </si>
@@ -38,12 +48,18 @@
   <si>
     <t>Acq N°5</t>
   </si>
+  <si>
+    <t>Pop 1 int:</t>
+  </si>
+  <si>
+    <t>Av</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +96,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -126,12 +147,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -158,14 +179,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -192,6 +214,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -367,16 +390,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T255"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T254"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X248" sqref="X248"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +430,11 @@
       <c r="S1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -469,8 +495,14 @@
       <c r="T2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2">
+        <v>0.1</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.10473200000000001</v>
       </c>
@@ -531,8 +563,14 @@
       <c r="T3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3">
+        <v>0.10473200000000001</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.10968799999999999</v>
       </c>
@@ -593,8 +631,14 @@
       <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4">
+        <v>0.10968799999999999</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.114879</v>
       </c>
@@ -655,8 +699,21 @@
       <c r="T5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5">
+        <v>0.114879</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5">
+        <f>AVERAGE(B88,D85,F77,H97,J89,P70)</f>
+        <v>0.13205772811939412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.12031500000000001</v>
       </c>
@@ -717,8 +774,21 @@
       <c r="T6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6">
+        <v>0.12031500000000001</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>7</v>
+      </c>
+      <c r="X6">
+        <f>AVERAGE(B138,D137,F134,H142,J140,L135,N136,P135,R134,T134)</f>
+        <v>0.92076536312836343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.12600900000000001</v>
       </c>
@@ -779,8 +849,14 @@
       <c r="T7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7">
+        <v>0.12600900000000001</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.13197200000000001</v>
       </c>
@@ -841,8 +917,14 @@
       <c r="T8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8">
+        <v>0.13197200000000001</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.13821700000000001</v>
       </c>
@@ -903,8 +985,14 @@
       <c r="T9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9">
+        <v>0.13821700000000001</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.144758</v>
       </c>
@@ -965,8 +1053,14 @@
       <c r="T10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10">
+        <v>0.144758</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.15160799999999999</v>
       </c>
@@ -1027,8 +1121,14 @@
       <c r="T11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11">
+        <v>0.15160799999999999</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.15878300000000001</v>
       </c>
@@ -1089,8 +1189,14 @@
       <c r="T12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12">
+        <v>0.15878300000000001</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.166297</v>
       </c>
@@ -1151,8 +1257,14 @@
       <c r="T13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13">
+        <v>0.166297</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.17416599999999999</v>
       </c>
@@ -1213,8 +1325,14 @@
       <c r="T14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14">
+        <v>0.17416599999999999</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.18240799999999999</v>
       </c>
@@ -1275,8 +1393,14 @@
       <c r="T15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15">
+        <v>0.18240799999999999</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.19103999999999999</v>
       </c>
@@ -1337,8 +1461,14 @@
       <c r="T16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16">
+        <v>0.19103999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.20008100000000001</v>
       </c>
@@ -1399,8 +1529,14 @@
       <c r="T17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="U17">
+        <v>0.20008100000000001</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.20954900000000001</v>
       </c>
@@ -1461,8 +1597,14 @@
       <c r="T18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="U18">
+        <v>0.20954900000000001</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.21946499999999999</v>
       </c>
@@ -1523,8 +1665,14 @@
       <c r="T19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="U19">
+        <v>0.21946499999999999</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0.229851</v>
       </c>
@@ -1585,8 +1733,14 @@
       <c r="T20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="U20">
+        <v>0.229851</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0.240728</v>
       </c>
@@ -1647,8 +1801,14 @@
       <c r="T21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="U21">
+        <v>0.240728</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0.25211899999999998</v>
       </c>
@@ -1709,8 +1869,14 @@
       <c r="T22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="U22">
+        <v>0.25211899999999998</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>0.26405000000000001</v>
       </c>
@@ -1771,8 +1937,14 @@
       <c r="T23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="U23">
+        <v>0.26405000000000001</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>0.27654600000000001</v>
       </c>
@@ -1833,8 +2005,14 @@
       <c r="T24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="U24">
+        <v>0.27654600000000001</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0.28963299999999997</v>
       </c>
@@ -1895,8 +2073,14 @@
       <c r="T25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="U25">
+        <v>0.28963299999999997</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.30333900000000003</v>
       </c>
@@ -1957,8 +2141,14 @@
       <c r="T26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="U26">
+        <v>0.30333900000000003</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.317693</v>
       </c>
@@ -2019,8 +2209,14 @@
       <c r="T27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="U27">
+        <v>0.317693</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0.33272699999999999</v>
       </c>
@@ -2081,8 +2277,14 @@
       <c r="T28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="U28">
+        <v>0.33272699999999999</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>0.34847299999999998</v>
       </c>
@@ -2143,8 +2345,14 @@
       <c r="T29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="U29">
+        <v>0.34847299999999998</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.36496299999999998</v>
       </c>
@@ -2205,8 +2413,14 @@
       <c r="T30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="U30">
+        <v>0.36496299999999998</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.38223400000000002</v>
       </c>
@@ -2267,8 +2481,14 @@
       <c r="T31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="U31">
+        <v>0.38223400000000002</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.40032200000000001</v>
       </c>
@@ -2329,8 +2549,14 @@
       <c r="T32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="U32">
+        <v>0.40032200000000001</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.41926600000000003</v>
       </c>
@@ -2391,8 +2617,14 @@
       <c r="T33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="U33">
+        <v>0.41926600000000003</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.43910700000000003</v>
       </c>
@@ -2453,8 +2685,14 @@
       <c r="T34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="U34">
+        <v>0.43910700000000003</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.45988600000000002</v>
       </c>
@@ -2515,8 +2753,14 @@
       <c r="T35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="U35">
+        <v>0.45988600000000002</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.48164899999999999</v>
       </c>
@@ -2577,8 +2821,14 @@
       <c r="T36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="U36">
+        <v>0.48164899999999999</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.50444199999999995</v>
       </c>
@@ -2639,8 +2889,14 @@
       <c r="T37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="U37">
+        <v>0.50444199999999995</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.52831300000000003</v>
       </c>
@@ -2701,8 +2957,14 @@
       <c r="T38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="U38">
+        <v>0.52831300000000003</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.55331399999999997</v>
       </c>
@@ -2763,8 +3025,14 @@
       <c r="T39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:20">
+      <c r="U39">
+        <v>0.55331399999999997</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.57949799999999996</v>
       </c>
@@ -2825,8 +3093,14 @@
       <c r="T40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:20">
+      <c r="U40">
+        <v>0.57949799999999996</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0.60692199999999996</v>
       </c>
@@ -2887,8 +3161,14 @@
       <c r="T41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="U41">
+        <v>0.60692199999999996</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0.63564200000000004</v>
       </c>
@@ -2949,8 +3229,14 @@
       <c r="T42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="U42">
+        <v>0.63564200000000004</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0.66572200000000004</v>
       </c>
@@ -3011,8 +3297,14 @@
       <c r="T43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:20">
+      <c r="U43">
+        <v>0.66572200000000004</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0.69722600000000001</v>
       </c>
@@ -3073,8 +3365,14 @@
       <c r="T44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:20">
+      <c r="U44">
+        <v>0.69722600000000001</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0.73021999999999998</v>
       </c>
@@ -3135,8 +3433,14 @@
       <c r="T45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:20">
+      <c r="U45">
+        <v>0.73021999999999998</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0.76477600000000001</v>
       </c>
@@ -3197,8 +3501,14 @@
       <c r="T46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20">
+      <c r="U46">
+        <v>0.76477600000000001</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0.80096699999999998</v>
       </c>
@@ -3259,8 +3569,14 @@
       <c r="T47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="U47">
+        <v>0.80096699999999998</v>
+      </c>
+      <c r="V47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0.83887</v>
       </c>
@@ -3321,8 +3637,14 @@
       <c r="T48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:20">
+      <c r="U48">
+        <v>0.83887</v>
+      </c>
+      <c r="V48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>0.87856699999999999</v>
       </c>
@@ -3383,8 +3705,14 @@
       <c r="T49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:20">
+      <c r="U49">
+        <v>0.87856699999999999</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0.92014300000000004</v>
       </c>
@@ -3445,8 +3773,14 @@
       <c r="T50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:20">
+      <c r="U50">
+        <v>0.92014300000000004</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0.96368600000000004</v>
       </c>
@@ -3507,8 +3841,14 @@
       <c r="T51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:20">
+      <c r="U51">
+        <v>0.96368600000000004</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1.00929</v>
       </c>
@@ -3569,8 +3909,14 @@
       <c r="T52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:20">
+      <c r="U52">
+        <v>1.00929</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1.0570520000000001</v>
       </c>
@@ -3631,8 +3977,14 @@
       <c r="T53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:20">
+      <c r="U53">
+        <v>1.0570520000000001</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1.1070739999999999</v>
       </c>
@@ -3693,8 +4045,14 @@
       <c r="T54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:20">
+      <c r="U54">
+        <v>1.1070739999999999</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1.1594629999999999</v>
       </c>
@@ -3755,8 +4113,14 @@
       <c r="T55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:20">
+      <c r="U55">
+        <v>1.1594629999999999</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1.214332</v>
       </c>
@@ -3817,8 +4181,14 @@
       <c r="T56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:20">
+      <c r="U56">
+        <v>1.214332</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1.2717970000000001</v>
       </c>
@@ -3879,8 +4249,14 @@
       <c r="T57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:20">
+      <c r="U57">
+        <v>1.2717970000000001</v>
+      </c>
+      <c r="V57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1.3319810000000001</v>
       </c>
@@ -3941,8 +4317,14 @@
       <c r="T58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:20">
+      <c r="U58">
+        <v>1.3319810000000001</v>
+      </c>
+      <c r="V58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1.3950130000000001</v>
       </c>
@@ -4003,8 +4385,14 @@
       <c r="T59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:20">
+      <c r="U59">
+        <v>1.3950130000000001</v>
+      </c>
+      <c r="V59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1.461028</v>
       </c>
@@ -4065,8 +4453,14 @@
       <c r="T60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:20">
+      <c r="U60">
+        <v>1.461028</v>
+      </c>
+      <c r="V60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1.5301670000000001</v>
       </c>
@@ -4127,8 +4521,14 @@
       <c r="T61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:20">
+      <c r="U61">
+        <v>1.5301670000000001</v>
+      </c>
+      <c r="V61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1.6025780000000001</v>
       </c>
@@ -4189,8 +4589,14 @@
       <c r="T62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:20">
+      <c r="U62">
+        <v>1.6025780000000001</v>
+      </c>
+      <c r="V62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1.6784159999999999</v>
       </c>
@@ -4251,8 +4657,14 @@
       <c r="T63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:20">
+      <c r="U63">
+        <v>1.6784159999999999</v>
+      </c>
+      <c r="V63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1.7578419999999999</v>
       </c>
@@ -4313,8 +4725,14 @@
       <c r="T64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:20">
+      <c r="U64">
+        <v>1.7578419999999999</v>
+      </c>
+      <c r="V64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1.841027</v>
       </c>
@@ -4375,8 +4793,14 @@
       <c r="T65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:20">
+      <c r="U65">
+        <v>1.841027</v>
+      </c>
+      <c r="V65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1.9281489999999999</v>
       </c>
@@ -4437,8 +4861,14 @@
       <c r="T66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:20">
+      <c r="U66">
+        <v>1.9281489999999999</v>
+      </c>
+      <c r="V66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2.019393</v>
       </c>
@@ -4499,8 +4929,14 @@
       <c r="T67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:20">
+      <c r="U67">
+        <v>2.019393</v>
+      </c>
+      <c r="V67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2.1149550000000001</v>
       </c>
@@ -4561,8 +4997,14 @@
       <c r="T68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:20">
+      <c r="U68">
+        <v>2.1149550000000001</v>
+      </c>
+      <c r="V68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2.2150400000000001</v>
       </c>
@@ -4623,8 +5065,14 @@
       <c r="T69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:20">
+      <c r="U69">
+        <v>2.2150400000000001</v>
+      </c>
+      <c r="V69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2.3198599999999998</v>
       </c>
@@ -4685,8 +5133,14 @@
       <c r="T70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:20">
+      <c r="U70">
+        <v>2.3198599999999998</v>
+      </c>
+      <c r="V70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2.4296410000000002</v>
       </c>
@@ -4747,8 +5201,14 @@
       <c r="T71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:20">
+      <c r="U71">
+        <v>2.4296410000000002</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2.5446170000000001</v>
       </c>
@@ -4809,8 +5269,14 @@
       <c r="T72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:20">
+      <c r="U72">
+        <v>2.5446170000000001</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2.6650339999999999</v>
       </c>
@@ -4871,8 +5337,14 @@
       <c r="T73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:20">
+      <c r="U73">
+        <v>2.6650339999999999</v>
+      </c>
+      <c r="V73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2.79115</v>
       </c>
@@ -4933,8 +5405,14 @@
       <c r="T74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:20">
+      <c r="U74">
+        <v>2.79115</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2.9232330000000002</v>
       </c>
@@ -4995,8 +5473,14 @@
       <c r="T75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:20">
+      <c r="U75">
+        <v>2.9232330000000002</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>3.0615670000000001</v>
       </c>
@@ -5057,8 +5541,14 @@
       <c r="T76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:20">
+      <c r="U76">
+        <v>3.0615670000000001</v>
+      </c>
+      <c r="V76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>3.2064469999999998</v>
       </c>
@@ -5119,8 +5609,14 @@
       <c r="T77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:20">
+      <c r="U77">
+        <v>3.2064469999999998</v>
+      </c>
+      <c r="V77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>3.3581829999999999</v>
       </c>
@@ -5181,8 +5677,14 @@
       <c r="T78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:20">
+      <c r="U78">
+        <v>3.3581829999999999</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>3.5171000000000001</v>
       </c>
@@ -5243,8 +5745,14 @@
       <c r="T79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:20">
+      <c r="U79">
+        <v>3.5171000000000001</v>
+      </c>
+      <c r="V79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>3.6835369999999998</v>
       </c>
@@ -5305,8 +5813,14 @@
       <c r="T80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:20">
+      <c r="U80">
+        <v>3.6835369999999998</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>3.85785</v>
       </c>
@@ -5367,8 +5881,14 @@
       <c r="T81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:20">
+      <c r="U81">
+        <v>3.85785</v>
+      </c>
+      <c r="V81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>4.0404119999999999</v>
       </c>
@@ -5429,8 +5949,14 @@
       <c r="T82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:20">
+      <c r="U82">
+        <v>4.0404119999999999</v>
+      </c>
+      <c r="V82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>4.2316140000000004</v>
       </c>
@@ -5491,8 +6017,14 @@
       <c r="T83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:20">
+      <c r="U83">
+        <v>4.2316140000000004</v>
+      </c>
+      <c r="V83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>4.4318629999999999</v>
       </c>
@@ -5553,8 +6085,14 @@
       <c r="T84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:20">
+      <c r="U84">
+        <v>4.4318629999999999</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>4.6415889999999997</v>
       </c>
@@ -5615,8 +6153,14 @@
       <c r="T85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:20">
+      <c r="U85">
+        <v>4.6415889999999997</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>4.8612390000000003</v>
       </c>
@@ -5677,8 +6221,15 @@
       <c r="T86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:20">
+      <c r="U86">
+        <v>4.8612390000000003</v>
+      </c>
+      <c r="V86">
+        <f>X5</f>
+        <v>0.13205772811939412</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>5.0912839999999999</v>
       </c>
@@ -5739,8 +6290,14 @@
       <c r="T87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:20">
+      <c r="U87">
+        <v>5.0912839999999999</v>
+      </c>
+      <c r="V87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>5.3322149999999997</v>
       </c>
@@ -5801,8 +6358,14 @@
       <c r="T88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:20">
+      <c r="U88">
+        <v>5.3322149999999997</v>
+      </c>
+      <c r="V88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>5.5845469999999997</v>
       </c>
@@ -5863,8 +6426,14 @@
       <c r="T89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:20">
+      <c r="U89">
+        <v>5.5845469999999997</v>
+      </c>
+      <c r="V89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>5.8488199999999999</v>
       </c>
@@ -5925,8 +6494,14 @@
       <c r="T90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:20">
+      <c r="U90">
+        <v>5.8488199999999999</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>6.1255990000000002</v>
       </c>
@@ -5987,8 +6562,14 @@
       <c r="T91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:20">
+      <c r="U91">
+        <v>6.1255990000000002</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>6.415476</v>
       </c>
@@ -6049,8 +6630,14 @@
       <c r="T92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:20">
+      <c r="U92">
+        <v>6.415476</v>
+      </c>
+      <c r="V92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>6.7190709999999996</v>
       </c>
@@ -6111,8 +6698,14 @@
       <c r="T93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:20">
+      <c r="U93">
+        <v>6.7190709999999996</v>
+      </c>
+      <c r="V93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>7.0370330000000001</v>
       </c>
@@ -6173,8 +6766,14 @@
       <c r="T94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:20">
+      <c r="U94">
+        <v>7.0370330000000001</v>
+      </c>
+      <c r="V94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>7.3700409999999996</v>
       </c>
@@ -6235,8 +6834,14 @@
       <c r="T95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:20">
+      <c r="U95">
+        <v>7.3700409999999996</v>
+      </c>
+      <c r="V95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>7.718807</v>
       </c>
@@ -6297,8 +6902,14 @@
       <c r="T96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:20">
+      <c r="U96">
+        <v>7.718807</v>
+      </c>
+      <c r="V96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>8.0840789999999991</v>
       </c>
@@ -6359,8 +6970,14 @@
       <c r="T97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:20">
+      <c r="U97">
+        <v>8.0840789999999991</v>
+      </c>
+      <c r="V97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>8.4666350000000001</v>
       </c>
@@ -6421,8 +7038,14 @@
       <c r="T98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:20">
+      <c r="U98">
+        <v>8.4666350000000001</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>8.8672950000000004</v>
       </c>
@@ -6483,8 +7106,14 @@
       <c r="T99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:20">
+      <c r="U99">
+        <v>8.8672950000000004</v>
+      </c>
+      <c r="V99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>9.2869150000000005</v>
       </c>
@@ -6545,8 +7174,14 @@
       <c r="T100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:20">
+      <c r="U100">
+        <v>9.2869150000000005</v>
+      </c>
+      <c r="V100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>9.7263929999999998</v>
       </c>
@@ -6607,8 +7242,14 @@
       <c r="T101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:20">
+      <c r="U101">
+        <v>9.7263929999999998</v>
+      </c>
+      <c r="V101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>10.186667</v>
       </c>
@@ -6669,8 +7310,14 @@
       <c r="T102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:20">
+      <c r="U102">
+        <v>10.186667</v>
+      </c>
+      <c r="V102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>10.668723</v>
       </c>
@@ -6731,8 +7378,14 @@
       <c r="T103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:20">
+      <c r="U103">
+        <v>10.668723</v>
+      </c>
+      <c r="V103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>11.173591</v>
       </c>
@@ -6793,8 +7446,14 @@
       <c r="T104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:20">
+      <c r="U104">
+        <v>11.173591</v>
+      </c>
+      <c r="V104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>11.702349999999999</v>
       </c>
@@ -6855,8 +7514,14 @@
       <c r="T105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:20">
+      <c r="U105">
+        <v>11.702349999999999</v>
+      </c>
+      <c r="V105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>12.256131999999999</v>
       </c>
@@ -6917,8 +7582,14 @@
       <c r="T106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:20">
+      <c r="U106">
+        <v>12.256131999999999</v>
+      </c>
+      <c r="V106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>12.836119</v>
       </c>
@@ -6979,8 +7650,14 @@
       <c r="T107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:20">
+      <c r="U107">
+        <v>12.836119</v>
+      </c>
+      <c r="V107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>13.443553</v>
       </c>
@@ -7041,8 +7718,14 @@
       <c r="T108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:20">
+      <c r="U108">
+        <v>13.443553</v>
+      </c>
+      <c r="V108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>14.079732</v>
       </c>
@@ -7103,8 +7786,14 @@
       <c r="T109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:20">
+      <c r="U109">
+        <v>14.079732</v>
+      </c>
+      <c r="V109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>14.746015999999999</v>
       </c>
@@ -7165,8 +7854,14 @@
       <c r="T110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:20">
+      <c r="U110">
+        <v>14.746015999999999</v>
+      </c>
+      <c r="V110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>15.44383</v>
       </c>
@@ -7227,8 +7922,14 @@
       <c r="T111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:20">
+      <c r="U111">
+        <v>15.44383</v>
+      </c>
+      <c r="V111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>16.174666999999999</v>
       </c>
@@ -7289,8 +7990,14 @@
       <c r="T112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:20">
+      <c r="U112">
+        <v>16.174666999999999</v>
+      </c>
+      <c r="V112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>16.940087999999999</v>
       </c>
@@ -7351,8 +8058,14 @@
       <c r="T113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:20">
+      <c r="U113">
+        <v>16.940087999999999</v>
+      </c>
+      <c r="V113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>17.741731000000001</v>
       </c>
@@ -7413,8 +8126,14 @@
       <c r="T114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:20">
+      <c r="U114">
+        <v>17.741731000000001</v>
+      </c>
+      <c r="V114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>18.581309000000001</v>
       </c>
@@ -7475,8 +8194,14 @@
       <c r="T115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:20">
+      <c r="U115">
+        <v>18.581309000000001</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>19.460618</v>
       </c>
@@ -7537,8 +8262,14 @@
       <c r="T116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:20">
+      <c r="U116">
+        <v>19.460618</v>
+      </c>
+      <c r="V116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>20.381537999999999</v>
       </c>
@@ -7599,8 +8330,14 @@
       <c r="T117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:20">
+      <c r="U117">
+        <v>20.381537999999999</v>
+      </c>
+      <c r="V117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>21.346038</v>
       </c>
@@ -7661,8 +8398,14 @@
       <c r="T118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:20">
+      <c r="U118">
+        <v>21.346038</v>
+      </c>
+      <c r="V118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>22.356179999999998</v>
       </c>
@@ -7723,8 +8466,14 @@
       <c r="T119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:20">
+      <c r="U119">
+        <v>22.356179999999998</v>
+      </c>
+      <c r="V119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>23.414124000000001</v>
       </c>
@@ -7785,8 +8534,14 @@
       <c r="T120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:20">
+      <c r="U120">
+        <v>23.414124000000001</v>
+      </c>
+      <c r="V120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>24.522131999999999</v>
       </c>
@@ -7847,8 +8602,14 @@
       <c r="T121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:20">
+      <c r="U121">
+        <v>24.522131999999999</v>
+      </c>
+      <c r="V121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>25.682573999999999</v>
       </c>
@@ -7909,8 +8670,14 @@
       <c r="T122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:20">
+      <c r="U122">
+        <v>25.682573999999999</v>
+      </c>
+      <c r="V122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>26.897931</v>
       </c>
@@ -7971,8 +8738,14 @@
       <c r="T123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:20">
+      <c r="U123">
+        <v>26.897931</v>
+      </c>
+      <c r="V123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>28.170801000000001</v>
       </c>
@@ -8033,8 +8806,14 @@
       <c r="T124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:20">
+      <c r="U124">
+        <v>28.170801000000001</v>
+      </c>
+      <c r="V124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>29.503906000000001</v>
       </c>
@@ -8095,8 +8874,14 @@
       <c r="T125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:20">
+      <c r="U125">
+        <v>29.503906000000001</v>
+      </c>
+      <c r="V125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>30.900096999999999</v>
       </c>
@@ -8157,8 +8942,14 @@
       <c r="T126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:20">
+      <c r="U126">
+        <v>30.900096999999999</v>
+      </c>
+      <c r="V126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>32.362358</v>
       </c>
@@ -8219,8 +9010,14 @@
       <c r="T127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:20">
+      <c r="U127">
+        <v>32.362358</v>
+      </c>
+      <c r="V127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>33.893816999999999</v>
       </c>
@@ -8281,8 +9078,14 @@
       <c r="T128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:20">
+      <c r="U128">
+        <v>33.893816999999999</v>
+      </c>
+      <c r="V128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>35.497748000000001</v>
       </c>
@@ -8343,8 +9146,14 @@
       <c r="T129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:20">
+      <c r="U129">
+        <v>35.497748000000001</v>
+      </c>
+      <c r="V129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>37.177581000000004</v>
       </c>
@@ -8405,8 +9214,14 @@
       <c r="T130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:20">
+      <c r="U130">
+        <v>37.177581000000004</v>
+      </c>
+      <c r="V130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>38.936906999999998</v>
       </c>
@@ -8467,8 +9282,14 @@
       <c r="T131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:20">
+      <c r="U131">
+        <v>38.936906999999998</v>
+      </c>
+      <c r="V131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>40.779488000000001</v>
       </c>
@@ -8529,8 +9350,14 @@
       <c r="T132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:20">
+      <c r="U132">
+        <v>40.779488000000001</v>
+      </c>
+      <c r="V132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>42.709263999999997</v>
       </c>
@@ -8591,8 +9418,14 @@
       <c r="T133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:20">
+      <c r="U133">
+        <v>42.709263999999997</v>
+      </c>
+      <c r="V133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>44.730362</v>
       </c>
@@ -8653,8 +9486,14 @@
       <c r="T134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:20">
+      <c r="U134">
+        <v>44.730362</v>
+      </c>
+      <c r="V134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>46.847102</v>
       </c>
@@ -8715,8 +9554,14 @@
       <c r="T135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:20">
+      <c r="U135">
+        <v>46.847102</v>
+      </c>
+      <c r="V135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>49.064011000000001</v>
       </c>
@@ -8777,8 +9622,14 @@
       <c r="T136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:20">
+      <c r="U136">
+        <v>49.064011000000001</v>
+      </c>
+      <c r="V136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>51.385829999999999</v>
       </c>
@@ -8839,8 +9690,15 @@
       <c r="T137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:20">
+      <c r="U137">
+        <v>51.385829999999999</v>
+      </c>
+      <c r="V137">
+        <f>X6</f>
+        <v>0.92076536312836343</v>
+      </c>
+    </row>
+    <row r="138" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>53.817521999999997</v>
       </c>
@@ -8901,8 +9759,14 @@
       <c r="T138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:20">
+      <c r="U138">
+        <v>53.817521999999997</v>
+      </c>
+      <c r="V138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>56.364286999999997</v>
       </c>
@@ -8963,8 +9827,14 @@
       <c r="T139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:20">
+      <c r="U139">
+        <v>56.364286999999997</v>
+      </c>
+      <c r="V139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>59.031570000000002</v>
       </c>
@@ -9025,8 +9895,14 @@
       <c r="T140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:20">
+      <c r="U140">
+        <v>59.031570000000002</v>
+      </c>
+      <c r="V140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>61.825076000000003</v>
       </c>
@@ -9087,8 +9963,14 @@
       <c r="T141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:20">
+      <c r="U141">
+        <v>61.825076000000003</v>
+      </c>
+      <c r="V141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>64.750776000000002</v>
       </c>
@@ -9149,8 +10031,14 @@
       <c r="T142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:20">
+      <c r="U142">
+        <v>64.750776000000002</v>
+      </c>
+      <c r="V142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>67.814926999999997</v>
       </c>
@@ -9211,8 +10099,14 @@
       <c r="T143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:20">
+      <c r="U143">
+        <v>67.814926999999997</v>
+      </c>
+      <c r="V143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>71.024080999999995</v>
       </c>
@@ -9273,8 +10167,14 @@
       <c r="T144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:20">
+      <c r="U144">
+        <v>71.024080999999995</v>
+      </c>
+      <c r="V144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>74.385098999999997</v>
       </c>
@@ -9335,8 +10235,14 @@
       <c r="T145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:20">
+      <c r="U145">
+        <v>74.385098999999997</v>
+      </c>
+      <c r="V145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>77.905167000000006</v>
       </c>
@@ -9397,8 +10303,14 @@
       <c r="T146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:20">
+      <c r="U146">
+        <v>77.905167000000006</v>
+      </c>
+      <c r="V146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>81.591813999999999</v>
       </c>
@@ -9459,8 +10371,14 @@
       <c r="T147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:20">
+      <c r="U147">
+        <v>81.591813999999999</v>
+      </c>
+      <c r="V147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>85.452920000000006</v>
       </c>
@@ -9521,8 +10439,14 @@
       <c r="T148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:20">
+      <c r="U148">
+        <v>85.452920000000006</v>
+      </c>
+      <c r="V148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>89.496742999999995</v>
       </c>
@@ -9583,8 +10507,14 @@
       <c r="T149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:20">
+      <c r="U149">
+        <v>89.496742999999995</v>
+      </c>
+      <c r="V149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>93.731927999999996</v>
       </c>
@@ -9645,8 +10575,14 @@
       <c r="T150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:20">
+      <c r="U150">
+        <v>93.731927999999996</v>
+      </c>
+      <c r="V150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>98.167531999999994</v>
       </c>
@@ -9707,8 +10643,14 @@
       <c r="T151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:20">
+      <c r="U151">
+        <v>98.167531999999994</v>
+      </c>
+      <c r="V151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>102.81303800000001</v>
       </c>
@@ -9769,8 +10711,14 @@
       <c r="T152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:20">
+      <c r="U152">
+        <v>102.81303800000001</v>
+      </c>
+      <c r="V152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>107.67838</v>
       </c>
@@ -9831,8 +10779,14 @@
       <c r="T153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:20">
+      <c r="U153">
+        <v>107.67838</v>
+      </c>
+      <c r="V153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>112.773961</v>
       </c>
@@ -9893,8 +10847,14 @@
       <c r="T154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:20">
+      <c r="U154">
+        <v>112.773961</v>
+      </c>
+      <c r="V154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>118.110676</v>
       </c>
@@ -9955,8 +10915,14 @@
       <c r="T155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:20">
+      <c r="U155">
+        <v>118.110676</v>
+      </c>
+      <c r="V155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>123.69993700000001</v>
       </c>
@@ -10017,8 +10983,14 @@
       <c r="T156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:20">
+      <c r="U156">
+        <v>123.69993700000001</v>
+      </c>
+      <c r="V156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>129.55369400000001</v>
       </c>
@@ -10079,8 +11051,14 @@
       <c r="T157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:20">
+      <c r="U157">
+        <v>129.55369400000001</v>
+      </c>
+      <c r="V157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>135.68446299999999</v>
       </c>
@@ -10141,8 +11119,14 @@
       <c r="T158">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:20">
+      <c r="U158">
+        <v>135.68446299999999</v>
+      </c>
+      <c r="V158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>142.10535400000001</v>
       </c>
@@ -10203,8 +11187,14 @@
       <c r="T159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:20">
+      <c r="U159">
+        <v>142.10535400000001</v>
+      </c>
+      <c r="V159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>148.830096</v>
       </c>
@@ -10265,8 +11255,14 @@
       <c r="T160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:20">
+      <c r="U160">
+        <v>148.830096</v>
+      </c>
+      <c r="V160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>155.87306799999999</v>
       </c>
@@ -10327,8 +11323,14 @@
       <c r="T161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:20">
+      <c r="U161">
+        <v>155.87306799999999</v>
+      </c>
+      <c r="V161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>163.24932899999999</v>
       </c>
@@ -10389,8 +11391,14 @@
       <c r="T162">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:20">
+      <c r="U162">
+        <v>163.24932899999999</v>
+      </c>
+      <c r="V162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>170.97465099999999</v>
       </c>
@@ -10451,8 +11459,14 @@
       <c r="T163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:20">
+      <c r="U163">
+        <v>170.97465099999999</v>
+      </c>
+      <c r="V163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>179.06555299999999</v>
       </c>
@@ -10513,8 +11527,14 @@
       <c r="T164">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:20">
+      <c r="U164">
+        <v>179.06555299999999</v>
+      </c>
+      <c r="V164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>187.539334</v>
       </c>
@@ -10575,8 +11595,14 @@
       <c r="T165">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:20">
+      <c r="U165">
+        <v>187.539334</v>
+      </c>
+      <c r="V165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>196.41411299999999</v>
       </c>
@@ -10637,8 +11663,14 @@
       <c r="T166">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:20">
+      <c r="U166">
+        <v>196.41411299999999</v>
+      </c>
+      <c r="V166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>205.708867</v>
       </c>
@@ -10699,8 +11731,14 @@
       <c r="T167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:20">
+      <c r="U167">
+        <v>205.708867</v>
+      </c>
+      <c r="V167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>215.44346899999999</v>
       </c>
@@ -10761,8 +11799,14 @@
       <c r="T168">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:20">
+      <c r="U168">
+        <v>215.44346899999999</v>
+      </c>
+      <c r="V168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>225.638734</v>
       </c>
@@ -10823,8 +11867,14 @@
       <c r="T169">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:20">
+      <c r="U169">
+        <v>225.638734</v>
+      </c>
+      <c r="V169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>236.316462</v>
       </c>
@@ -10885,8 +11935,14 @@
       <c r="T170">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:20">
+      <c r="U170">
+        <v>236.316462</v>
+      </c>
+      <c r="V170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>247.499484</v>
       </c>
@@ -10947,8 +12003,14 @@
       <c r="T171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:20">
+      <c r="U171">
+        <v>247.499484</v>
+      </c>
+      <c r="V171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>259.21171099999998</v>
       </c>
@@ -11009,8 +12071,14 @@
       <c r="T172">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:20">
+      <c r="U172">
+        <v>259.21171099999998</v>
+      </c>
+      <c r="V172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>271.47818699999999</v>
       </c>
@@ -11071,8 +12139,14 @@
       <c r="T173">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:20">
+      <c r="U173">
+        <v>271.47818699999999</v>
+      </c>
+      <c r="V173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>284.32513999999998</v>
       </c>
@@ -11133,8 +12207,14 @@
       <c r="T174">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:20">
+      <c r="U174">
+        <v>284.32513999999998</v>
+      </c>
+      <c r="V174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>297.78003899999999</v>
       </c>
@@ -11195,8 +12275,14 @@
       <c r="T175">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:20">
+      <c r="U175">
+        <v>297.78003899999999</v>
+      </c>
+      <c r="V175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>311.87165399999998</v>
       </c>
@@ -11257,8 +12343,14 @@
       <c r="T176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:20">
+      <c r="U176">
+        <v>311.87165399999998</v>
+      </c>
+      <c r="V176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>326.63011599999999</v>
       </c>
@@ -11319,8 +12411,14 @@
       <c r="T177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:20">
+      <c r="U177">
+        <v>326.63011599999999</v>
+      </c>
+      <c r="V177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>342.08698099999998</v>
       </c>
@@ -11381,8 +12479,14 @@
       <c r="T178">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:20">
+      <c r="U178">
+        <v>342.08698099999998</v>
+      </c>
+      <c r="V178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>358.27529900000002</v>
       </c>
@@ -11443,8 +12547,14 @@
       <c r="T179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:20">
+      <c r="U179">
+        <v>358.27529900000002</v>
+      </c>
+      <c r="V179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>375.22968500000002</v>
       </c>
@@ -11505,8 +12615,14 @@
       <c r="T180">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:20">
+      <c r="U180">
+        <v>375.22968500000002</v>
+      </c>
+      <c r="V180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>392.98638999999997</v>
       </c>
@@ -11567,8 +12683,14 @@
       <c r="T181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:20">
+      <c r="U181">
+        <v>392.98638999999997</v>
+      </c>
+      <c r="V181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>411.58338199999997</v>
       </c>
@@ -11629,8 +12751,14 @@
       <c r="T182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:20">
+      <c r="U182">
+        <v>411.58338199999997</v>
+      </c>
+      <c r="V182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>431.06042500000001</v>
       </c>
@@ -11691,8 +12819,14 @@
       <c r="T183">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:20">
+      <c r="U183">
+        <v>431.06042500000001</v>
+      </c>
+      <c r="V183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>451.45916499999998</v>
       </c>
@@ -11753,8 +12887,14 @@
       <c r="T184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:20">
+      <c r="U184">
+        <v>451.45916499999998</v>
+      </c>
+      <c r="V184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>472.82321899999999</v>
       </c>
@@ -11815,8 +12955,14 @@
       <c r="T185">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:20">
+      <c r="U185">
+        <v>472.82321899999999</v>
+      </c>
+      <c r="V185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>495.19826699999999</v>
       </c>
@@ -11877,8 +13023,14 @@
       <c r="T186">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:20">
+      <c r="U186">
+        <v>495.19826699999999</v>
+      </c>
+      <c r="V186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>518.63215300000002</v>
       </c>
@@ -11939,8 +13091,14 @@
       <c r="T187">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:20">
+      <c r="U187">
+        <v>518.63215300000002</v>
+      </c>
+      <c r="V187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>543.174982</v>
       </c>
@@ -12001,8 +13159,14 @@
       <c r="T188">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:20">
+      <c r="U188">
+        <v>543.174982</v>
+      </c>
+      <c r="V188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>568.879233</v>
       </c>
@@ -12063,8 +13227,14 @@
       <c r="T189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:20">
+      <c r="U189">
+        <v>568.879233</v>
+      </c>
+      <c r="V189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>595.79986699999995</v>
       </c>
@@ -12125,8 +13295,14 @@
       <c r="T190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:20">
+      <c r="U190">
+        <v>595.79986699999995</v>
+      </c>
+      <c r="V190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>623.99444400000004</v>
       </c>
@@ -12187,8 +13363,14 @@
       <c r="T191">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:20">
+      <c r="U191">
+        <v>623.99444400000004</v>
+      </c>
+      <c r="V191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>653.52325199999996</v>
       </c>
@@ -12249,8 +13431,14 @@
       <c r="T192">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:20">
+      <c r="U192">
+        <v>653.52325199999996</v>
+      </c>
+      <c r="V192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>684.44942900000001</v>
       </c>
@@ -12311,8 +13499,14 @@
       <c r="T193">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:20">
+      <c r="U193">
+        <v>684.44942900000001</v>
+      </c>
+      <c r="V193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>716.83910100000003</v>
       </c>
@@ -12373,8 +13567,14 @@
       <c r="T194">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:20">
+      <c r="U194">
+        <v>716.83910100000003</v>
+      </c>
+      <c r="V194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>750.76152500000001</v>
       </c>
@@ -12435,8 +13635,14 @@
       <c r="T195">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:20">
+      <c r="U195">
+        <v>750.76152500000001</v>
+      </c>
+      <c r="V195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>786.28923399999996</v>
       </c>
@@ -12497,8 +13703,14 @@
       <c r="T196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:20">
+      <c r="U196">
+        <v>786.28923399999996</v>
+      </c>
+      <c r="V196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>823.49819300000001</v>
       </c>
@@ -12559,8 +13771,14 @@
       <c r="T197">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:20">
+      <c r="U197">
+        <v>823.49819300000001</v>
+      </c>
+      <c r="V197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>862.46796300000005</v>
       </c>
@@ -12621,8 +13839,14 @@
       <c r="T198">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:20">
+      <c r="U198">
+        <v>862.46796300000005</v>
+      </c>
+      <c r="V198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>903.28186900000003</v>
       </c>
@@ -12683,8 +13907,14 @@
       <c r="T199">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:20">
+      <c r="U199">
+        <v>903.28186900000003</v>
+      </c>
+      <c r="V199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>946.02718100000004</v>
       </c>
@@ -12745,8 +13975,14 @@
       <c r="T200">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:20">
+      <c r="U200">
+        <v>946.02718100000004</v>
+      </c>
+      <c r="V200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>990.79529500000001</v>
       </c>
@@ -12807,8 +14043,14 @@
       <c r="T201">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:20">
+      <c r="U201">
+        <v>990.79529500000001</v>
+      </c>
+      <c r="V201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>1037.6819370000001</v>
       </c>
@@ -12869,8 +14111,14 @@
       <c r="T202">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:20">
+      <c r="U202">
+        <v>1037.6819370000001</v>
+      </c>
+      <c r="V202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>1086.7873589999999</v>
       </c>
@@ -12931,8 +14179,14 @@
       <c r="T203">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:20">
+      <c r="U203">
+        <v>1086.7873589999999</v>
+      </c>
+      <c r="V203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1138.216559</v>
       </c>
@@ -12993,8 +14247,14 @@
       <c r="T204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:20">
+      <c r="U204">
+        <v>1138.216559</v>
+      </c>
+      <c r="V204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1192.079504</v>
       </c>
@@ -13055,8 +14315,14 @@
       <c r="T205">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:20">
+      <c r="U205">
+        <v>1192.079504</v>
+      </c>
+      <c r="V205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>1248.4913630000001</v>
       </c>
@@ -13117,8 +14383,14 @@
       <c r="T206">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:20">
+      <c r="U206">
+        <v>1248.4913630000001</v>
+      </c>
+      <c r="V206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>1307.5727569999999</v>
       </c>
@@ -13179,8 +14451,14 @@
       <c r="T207">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:20">
+      <c r="U207">
+        <v>1307.5727569999999</v>
+      </c>
+      <c r="V207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>1369.450014</v>
       </c>
@@ -13241,8 +14519,14 @@
       <c r="T208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:20">
+      <c r="U208">
+        <v>1369.450014</v>
+      </c>
+      <c r="V208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>1434.255441</v>
       </c>
@@ -13303,8 +14587,14 @@
       <c r="T209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:20">
+      <c r="U209">
+        <v>1434.255441</v>
+      </c>
+      <c r="V209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>1502.1276049999999</v>
       </c>
@@ -13365,8 +14655,14 @@
       <c r="T210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:20">
+      <c r="U210">
+        <v>1502.1276049999999</v>
+      </c>
+      <c r="V210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>1573.2116309999999</v>
       </c>
@@ -13427,8 +14723,14 @@
       <c r="T211">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:20">
+      <c r="U211">
+        <v>1573.2116309999999</v>
+      </c>
+      <c r="V211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>1647.6595119999999</v>
       </c>
@@ -13489,8 +14791,14 @@
       <c r="T212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:20">
+      <c r="U212">
+        <v>1647.6595119999999</v>
+      </c>
+      <c r="V212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>1725.6304319999999</v>
       </c>
@@ -13551,8 +14859,14 @@
       <c r="T213">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:20">
+      <c r="U213">
+        <v>1725.6304319999999</v>
+      </c>
+      <c r="V213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>1807.291111</v>
       </c>
@@ -13613,8 +14927,14 @@
       <c r="T214">
         <v>0</v>
       </c>
-    </row>
-    <row r="215" spans="1:20">
+      <c r="U214">
+        <v>1807.291111</v>
+      </c>
+      <c r="V214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>1892.8161540000001</v>
       </c>
@@ -13675,8 +14995,14 @@
       <c r="T215">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:20">
+      <c r="U215">
+        <v>1892.8161540000001</v>
+      </c>
+      <c r="V215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>1982.3884330000001</v>
       </c>
@@ -13737,8 +15063,14 @@
       <c r="T216">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:20">
+      <c r="U216">
+        <v>1982.3884330000001</v>
+      </c>
+      <c r="V216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>2076.1994719999998</v>
       </c>
@@ -13799,8 +15131,14 @@
       <c r="T217">
         <v>0</v>
       </c>
-    </row>
-    <row r="218" spans="1:20">
+      <c r="U217">
+        <v>2076.1994719999998</v>
+      </c>
+      <c r="V217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>2174.4498589999998</v>
       </c>
@@ -13861,8 +15199,14 @@
       <c r="T218">
         <v>0</v>
       </c>
-    </row>
-    <row r="219" spans="1:20">
+      <c r="U218">
+        <v>2174.4498589999998</v>
+      </c>
+      <c r="V218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>2277.3496719999998</v>
       </c>
@@ -13923,8 +15267,14 @@
       <c r="T219">
         <v>0</v>
       </c>
-    </row>
-    <row r="220" spans="1:20">
+      <c r="U219">
+        <v>2277.3496719999998</v>
+      </c>
+      <c r="V219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>2385.118935</v>
       </c>
@@ -13985,8 +15335,14 @@
       <c r="T220">
         <v>0</v>
       </c>
-    </row>
-    <row r="221" spans="1:20">
+      <c r="U220">
+        <v>2385.118935</v>
+      </c>
+      <c r="V220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>2497.9880790000002</v>
       </c>
@@ -14047,8 +15403,14 @@
       <c r="T221">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:20">
+      <c r="U221">
+        <v>2497.9880790000002</v>
+      </c>
+      <c r="V221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>2616.1984419999999</v>
       </c>
@@ -14109,8 +15471,14 @@
       <c r="T222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:20">
+      <c r="U222">
+        <v>2616.1984419999999</v>
+      </c>
+      <c r="V222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>2740.0027839999998</v>
       </c>
@@ -14171,8 +15539,14 @@
       <c r="T223">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:20">
+      <c r="U223">
+        <v>2740.0027839999998</v>
+      </c>
+      <c r="V223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>2869.6658219999999</v>
       </c>
@@ -14233,8 +15607,14 @@
       <c r="T224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:20">
+      <c r="U224">
+        <v>2869.6658219999999</v>
+      </c>
+      <c r="V224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>3005.4648050000001</v>
       </c>
@@ -14295,8 +15675,14 @@
       <c r="T225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:20">
+      <c r="U225">
+        <v>3005.4648050000001</v>
+      </c>
+      <c r="V225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>3147.690098</v>
       </c>
@@ -14357,8 +15743,14 @@
       <c r="T226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:20">
+      <c r="U226">
+        <v>3147.690098</v>
+      </c>
+      <c r="V226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>3296.6458090000001</v>
       </c>
@@ -14419,8 +15811,14 @@
       <c r="T227">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:20">
+      <c r="U227">
+        <v>3296.6458090000001</v>
+      </c>
+      <c r="V227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>3452.6504359999999</v>
       </c>
@@ -14481,8 +15879,14 @@
       <c r="T228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:20">
+      <c r="U228">
+        <v>3452.6504359999999</v>
+      </c>
+      <c r="V228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>3616.03755</v>
       </c>
@@ -14543,8 +15947,14 @@
       <c r="T229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:20">
+      <c r="U229">
+        <v>3616.03755</v>
+      </c>
+      <c r="V229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>3787.1565070000001</v>
       </c>
@@ -14605,8 +16015,14 @@
       <c r="T230">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:20">
+      <c r="U230">
+        <v>3787.1565070000001</v>
+      </c>
+      <c r="V230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>3966.3731939999998</v>
       </c>
@@ -14667,8 +16083,14 @@
       <c r="T231">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:20">
+      <c r="U231">
+        <v>3966.3731939999998</v>
+      </c>
+      <c r="V231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>4154.0708139999997</v>
       </c>
@@ -14729,8 +16151,14 @@
       <c r="T232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:20">
+      <c r="U232">
+        <v>4154.0708139999997</v>
+      </c>
+      <c r="V232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>4350.6507030000002</v>
       </c>
@@ -14791,8 +16219,14 @@
       <c r="T233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:20">
+      <c r="U233">
+        <v>4350.6507030000002</v>
+      </c>
+      <c r="V233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>4556.5331910000004</v>
       </c>
@@ -14853,8 +16287,14 @@
       <c r="T234">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:20">
+      <c r="U234">
+        <v>4556.5331910000004</v>
+      </c>
+      <c r="V234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>4772.1584970000004</v>
       </c>
@@ -14915,8 +16355,14 @@
       <c r="T235">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:20">
+      <c r="U235">
+        <v>4772.1584970000004</v>
+      </c>
+      <c r="V235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>4997.987674</v>
       </c>
@@ -14977,8 +16423,14 @@
       <c r="T236">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:20">
+      <c r="U236">
+        <v>4997.987674</v>
+      </c>
+      <c r="V236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>5234.5035900000003</v>
       </c>
@@ -15039,8 +16491,14 @@
       <c r="T237">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:20">
+      <c r="U237">
+        <v>5234.5035900000003</v>
+      </c>
+      <c r="V237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>5482.2119670000002</v>
       </c>
@@ -15101,8 +16559,14 @@
       <c r="T238">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:20">
+      <c r="U238">
+        <v>5482.2119670000002</v>
+      </c>
+      <c r="V238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>5741.6424559999996</v>
       </c>
@@ -15163,8 +16627,14 @@
       <c r="T239">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:20">
+      <c r="U239">
+        <v>5741.6424559999996</v>
+      </c>
+      <c r="V239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>6013.3497740000003</v>
       </c>
@@ -15225,8 +16695,14 @@
       <c r="T240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:20">
+      <c r="U240">
+        <v>6013.3497740000003</v>
+      </c>
+      <c r="V240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>6297.9148880000002</v>
       </c>
@@ -15287,8 +16763,14 @@
       <c r="T241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:20">
+      <c r="U241">
+        <v>6297.9148880000002</v>
+      </c>
+      <c r="V241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>6595.9462569999996</v>
       </c>
@@ -15349,8 +16831,14 @@
       <c r="T242">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:20">
+      <c r="U242">
+        <v>6595.9462569999996</v>
+      </c>
+      <c r="V242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>6908.0811350000004</v>
       </c>
@@ -15411,8 +16899,14 @@
       <c r="T243">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:20">
+      <c r="U243">
+        <v>6908.0811350000004</v>
+      </c>
+      <c r="V243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>7234.9869319999998</v>
       </c>
@@ -15473,8 +16967,14 @@
       <c r="T244">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:20">
+      <c r="U244">
+        <v>7234.9869319999998</v>
+      </c>
+      <c r="V244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>7577.3626389999999</v>
       </c>
@@ -15535,8 +17035,14 @@
       <c r="T245">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:20">
+      <c r="U245">
+        <v>7577.3626389999999</v>
+      </c>
+      <c r="V245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>7935.9403270000003</v>
       </c>
@@ -15597,8 +17103,14 @@
       <c r="T246">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:20">
+      <c r="U246">
+        <v>7935.9403270000003</v>
+      </c>
+      <c r="V246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>8311.4867109999996</v>
       </c>
@@ -15659,8 +17171,14 @@
       <c r="T247">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:20">
+      <c r="U247">
+        <v>8311.4867109999996</v>
+      </c>
+      <c r="V247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>8704.8047869999991</v>
       </c>
@@ -15721,8 +17239,14 @@
       <c r="T248">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:20">
+      <c r="U248">
+        <v>8704.8047869999991</v>
+      </c>
+      <c r="V248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>9116.7355509999998</v>
       </c>
@@ -15783,8 +17307,14 @@
       <c r="T249">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:20">
+      <c r="U249">
+        <v>9116.7355509999998</v>
+      </c>
+      <c r="V249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>9548.1597970000003</v>
       </c>
@@ -15845,8 +17375,14 @@
       <c r="T250">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:20">
+      <c r="U250">
+        <v>9548.1597970000003</v>
+      </c>
+      <c r="V250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>10000</v>
       </c>
@@ -15907,8 +17443,14 @@
       <c r="T251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:20">
+      <c r="U251">
+        <v>10000</v>
+      </c>
+      <c r="V251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>1</v>
       </c>
@@ -15939,8 +17481,11 @@
       <c r="S252" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="253" spans="1:20">
+      <c r="U252" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>4.8612390000000003</v>
       </c>
@@ -16001,8 +17546,11 @@
       <c r="T253">
         <v>0.80775651521240899</v>
       </c>
-    </row>
-    <row r="254" spans="1:20">
+      <c r="U253">
+        <v>4.8612390000000003</v>
+      </c>
+    </row>
+    <row r="254" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>53.817521999999997</v>
       </c>
@@ -16048,8 +17596,11 @@
       <c r="S254" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="255" spans="1:20">
+      <c r="U254">
+        <v>53.817521999999997</v>
+      </c>
+    </row>
+    <row r="255" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>2</v>
       </c>
@@ -16063,6 +17614,9 @@
         <v>2</v>
       </c>
       <c r="I255" t="s">
+        <v>2</v>
+      </c>
+      <c r="U255" t="s">
         <v>2</v>
       </c>
     </row>
@@ -16072,24 +17626,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>